<commit_message>
Update to project name
I read it as "team name" at first, updated it appropirately
</commit_message>
<xml_diff>
--- a/Task List.xlsx
+++ b/Task List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\GitHub\BDAD_proj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6B73FF-EBB8-44B1-8C82-6D3F7B1E11DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D0E5CC-F824-488C-A5BE-B996E129B1A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-18120" yWindow="-16125" windowWidth="18240" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,9 +262,6 @@
     <t>7/22/2020</t>
   </si>
   <si>
-    <t>Team Lightning</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1) Alex Spence</t>
   </si>
   <si>
@@ -272,6 +269,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 3) Mike Urciuoli</t>
+  </si>
+  <si>
+    <t>Model-based AGI Prediction</t>
   </si>
 </sst>
 </file>
@@ -1017,12 +1017,96 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="11" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1053,15 +1137,6 @@
     <xf numFmtId="49" fontId="4" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1075,81 +1150,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2342,10 +2342,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:IV46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -2362,71 +2365,71 @@
   <sheetData>
     <row r="1" spans="1:7" ht="74.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="2"/>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="37"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="65"/>
     </row>
     <row r="2" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2"/>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="48" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="50"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="3" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2"/>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="53"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="36"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2"/>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="54" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="56"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="39"/>
     </row>
     <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="2"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="57" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="59"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="42"/>
     </row>
     <row r="6" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="42"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
     </row>
     <row r="7" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="2"/>
@@ -2452,22 +2455,22 @@
     <row r="8" spans="1:7" ht="28.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="42"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="30"/>
     </row>
     <row r="9" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="2"/>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="37"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="65"/>
     </row>
     <row r="10" spans="1:7" ht="44" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="2"/>
@@ -2490,19 +2493,19 @@
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="2"/>
-      <c r="B11" s="43">
+      <c r="B11" s="68">
         <v>2</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="67" t="s">
+      <c r="D11" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="69" t="s">
+      <c r="E11" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="71" t="s">
+      <c r="F11" s="55" t="s">
         <v>44</v>
       </c>
       <c r="G11" s="10" t="s">
@@ -2511,11 +2514,11 @@
     </row>
     <row r="12" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="2"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="72"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="56"/>
       <c r="G12" s="11"/>
     </row>
     <row r="13" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.5">
@@ -2542,33 +2545,33 @@
     <row r="14" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="42"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="30"/>
     </row>
     <row r="15" spans="1:7" ht="68" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A15" s="2"/>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="37"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="65"/>
     </row>
     <row r="16" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="2"/>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="37"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="65"/>
     </row>
     <row r="17" spans="1:7" ht="62.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A17" s="2"/>
@@ -2632,22 +2635,22 @@
     <row r="20" spans="1:7" ht="18.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="42"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="30"/>
     </row>
     <row r="21" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="2"/>
-      <c r="B21" s="39" t="s">
+      <c r="B21" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="37"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="65"/>
     </row>
     <row r="22" spans="1:7" ht="69.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" s="2"/>
@@ -2711,22 +2714,22 @@
     <row r="25" spans="1:7" ht="18.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="42"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="30"/>
     </row>
     <row r="26" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A26" s="2"/>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="35"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="37"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="65"/>
     </row>
     <row r="27" spans="1:7" ht="64.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A27" s="2"/>
@@ -2790,26 +2793,26 @@
     <row r="30" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="42"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="30"/>
     </row>
     <row r="31" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A31" s="2"/>
-      <c r="B31" s="47" t="s">
+      <c r="B31" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="35"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="37"/>
+      <c r="C31" s="63"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="65"/>
     </row>
     <row r="32" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A32" s="2"/>
-      <c r="B32" s="44" t="s">
+      <c r="B32" s="69" t="s">
         <v>55</v>
       </c>
       <c r="C32" s="16" t="s">
@@ -2828,7 +2831,7 @@
     </row>
     <row r="33" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A33" s="2"/>
-      <c r="B33" s="29"/>
+      <c r="B33" s="44"/>
       <c r="C33" s="16" t="s">
         <v>29</v>
       </c>
@@ -2845,7 +2848,7 @@
     </row>
     <row r="34" spans="1:7" ht="44.55" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A34" s="2"/>
-      <c r="B34" s="29"/>
+      <c r="B34" s="44"/>
       <c r="C34" s="16" t="s">
         <v>30</v>
       </c>
@@ -2862,7 +2865,7 @@
     </row>
     <row r="35" spans="1:7" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A35" s="2"/>
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="71" t="s">
         <v>31</v>
       </c>
       <c r="C35" s="17" t="s">
@@ -2881,7 +2884,7 @@
     </row>
     <row r="36" spans="1:7" ht="44.55" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A36" s="2"/>
-      <c r="B36" s="29"/>
+      <c r="B36" s="44"/>
       <c r="C36" s="17" t="s">
         <v>33</v>
       </c>
@@ -2898,7 +2901,7 @@
     </row>
     <row r="37" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A37" s="2"/>
-      <c r="B37" s="29"/>
+      <c r="B37" s="44"/>
       <c r="C37" s="17" t="s">
         <v>34</v>
       </c>
@@ -2915,7 +2918,7 @@
     </row>
     <row r="38" spans="1:7" ht="92.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A38" s="2"/>
-      <c r="B38" s="29"/>
+      <c r="B38" s="44"/>
       <c r="C38" s="17" t="s">
         <v>35</v>
       </c>
@@ -2932,7 +2935,7 @@
     </row>
     <row r="39" spans="1:7" ht="70.05" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A39" s="2"/>
-      <c r="B39" s="29"/>
+      <c r="B39" s="44"/>
       <c r="C39" s="17" t="s">
         <v>36</v>
       </c>
@@ -2949,7 +2952,7 @@
     </row>
     <row r="40" spans="1:7" ht="65.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A40" s="2"/>
-      <c r="B40" s="45" t="s">
+      <c r="B40" s="70" t="s">
         <v>37</v>
       </c>
       <c r="C40" s="19" t="s">
@@ -2968,7 +2971,7 @@
     </row>
     <row r="41" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A41" s="2"/>
-      <c r="B41" s="29"/>
+      <c r="B41" s="44"/>
       <c r="C41" s="19" t="s">
         <v>39</v>
       </c>
@@ -2985,7 +2988,7 @@
     </row>
     <row r="42" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A42" s="2"/>
-      <c r="B42" s="29"/>
+      <c r="B42" s="44"/>
       <c r="C42" s="19" t="s">
         <v>40</v>
       </c>
@@ -3003,18 +3006,18 @@
     <row r="43" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="42"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="30"/>
     </row>
     <row r="44" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A44" s="20"/>
-      <c r="B44" s="28" t="s">
+      <c r="B44" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="29"/>
+      <c r="C44" s="44"/>
       <c r="D44" s="21" t="s">
         <v>11</v>
       </c>
@@ -3028,8 +3031,8 @@
     </row>
     <row r="45" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A45" s="2"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="31"/>
+      <c r="B45" s="58"/>
+      <c r="C45" s="59"/>
       <c r="D45" s="23"/>
       <c r="E45" s="23"/>
       <c r="F45" s="23"/>
@@ -3037,8 +3040,8 @@
     </row>
     <row r="46" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A46" s="2"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="33"/>
+      <c r="B46" s="60"/>
+      <c r="C46" s="61"/>
       <c r="D46" s="25"/>
       <c r="E46" s="25"/>
       <c r="F46" s="25"/>
@@ -3048,6 +3051,21 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C46"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="B35:B39"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="C14:G14"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="C25:G25"/>
     <mergeCell ref="C30:G30"/>
@@ -3063,24 +3081,9 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="C6:G6"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C46"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B21:G21"/>
-    <mergeCell ref="C43:G43"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B40:B42"/>
-    <mergeCell ref="B35:B39"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B31:G31"/>
-    <mergeCell ref="C14:G14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup scale="46" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>